<commit_message>
fixing events data for complete merge
</commit_message>
<xml_diff>
--- a/Dataset/events_data/events_distances.xlsx
+++ b/Dataset/events_data/events_distances.xlsx
@@ -7324,34 +7324,34 @@
       </c>
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="n">
-        <v>4.69866</v>
+        <v>4.6989768</v>
       </c>
       <c r="O84" t="n">
-        <v>50.8687603</v>
+        <v>50.8691675</v>
       </c>
       <c r="P84" t="n">
-        <v>0.6216341623463915</v>
+        <v>0.5694821744253679</v>
       </c>
       <c r="Q84" t="n">
-        <v>0.9107465828270708</v>
+        <v>0.8585285922445823</v>
       </c>
       <c r="R84" t="n">
-        <v>0.6625663136780658</v>
+        <v>0.6111844965540491</v>
       </c>
       <c r="S84" t="n">
-        <v>0.763963680802656</v>
+        <v>0.7115405337077623</v>
       </c>
       <c r="T84" t="n">
-        <v>0.5871420207880528</v>
+        <v>0.5345547718793516</v>
       </c>
       <c r="U84" t="n">
-        <v>0.9599054194380933</v>
+        <v>0.9080543582212695</v>
       </c>
       <c r="V84" t="n">
-        <v>0.803443137798067</v>
+        <v>0.7522558810926905</v>
       </c>
       <c r="W84" t="n">
-        <v>1.12271967874532</v>
+        <v>1.071464322551493</v>
       </c>
     </row>
     <row r="85">
@@ -8630,34 +8630,34 @@
       </c>
       <c r="M100" t="inlineStr"/>
       <c r="N100" t="n">
-        <v>4.7151609</v>
+        <v>4.7154981</v>
       </c>
       <c r="O100" t="n">
-        <v>50.8818178</v>
+        <v>50.8810231</v>
       </c>
       <c r="P100" t="n">
-        <v>1.86989462531233</v>
+        <v>1.865621069025141</v>
       </c>
       <c r="Q100" t="n">
-        <v>1.694174841249579</v>
+        <v>1.702488508314046</v>
       </c>
       <c r="R100" t="n">
-        <v>1.859136149590306</v>
+        <v>1.857157925735173</v>
       </c>
       <c r="S100" t="n">
-        <v>1.773883429774273</v>
+        <v>1.775271755638189</v>
       </c>
       <c r="T100" t="n">
-        <v>1.884731409985826</v>
+        <v>1.878743932599191</v>
       </c>
       <c r="U100" t="n">
-        <v>1.679944698898566</v>
+        <v>1.691055065353639</v>
       </c>
       <c r="V100" t="n">
-        <v>1.782124989295925</v>
+        <v>1.786466456694267</v>
       </c>
       <c r="W100" t="n">
-        <v>1.626683574770327</v>
+        <v>1.646753321402385</v>
       </c>
     </row>
     <row r="101">

</xml_diff>